<commit_message>
Change month summary template
</commit_message>
<xml_diff>
--- a/app/excel-parser/part_summary_template.xlsx
+++ b/app/excel-parser/part_summary_template.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC Projects\parts-manager\app\excel-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parts-manager\app\excel-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24254FE4-1EC9-46D7-9A90-47B063E8A436}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC91C10C-9CCB-4355-810F-18F57060664D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17160" xr2:uid="{FC2DCB68-3284-4E8F-BCF9-6D03E2C75FB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC2DCB68-3284-4E8F-BCF9-6D03E2C75FB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
     <sheet name="Empty" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -87,9 +95,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="[$-415]mmm\ yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="[$-415]mmm\ yy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -268,7 +276,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
@@ -293,7 +301,7 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -314,7 +322,7 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,7 +348,7 @@
     <xf numFmtId="2" fontId="9" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -350,7 +358,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,7 +376,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,7 +392,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,18 +711,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783B91BC-1864-4740-9E15-7234E6DACB23}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:14" s="29" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28"/>
@@ -752,45 +755,6 @@
         <v>12</v>
       </c>
       <c r="N1" s="38"/>
-    </row>
-    <row r="2" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -802,7 +766,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:M1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix empty line at the begining after creation summary file
</commit_message>
<xml_diff>
--- a/app/excel-parser/part_summary_template.xlsx
+++ b/app/excel-parser/part_summary_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parts-manager\app\excel-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSC Projects\parts-manager\app\excel-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1194CD-9586-43F4-972E-0CFF4E967A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739C5158-0B32-4D5A-923E-B1DF9BC581AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC2DCB68-3284-4E8F-BCF9-6D03E2C75FB6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FC2DCB68-3284-4E8F-BCF9-6D03E2C75FB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
     <sheet name="Empty" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -92,8 +94,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="[$-415]mmm\ yy;@"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="[$-415]mmm\ yy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -234,10 +236,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -249,10 +251,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -262,104 +264,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -677,47 +675,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783B91BC-1864-4740-9E15-7234E6DACB23}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="C1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" s="20" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="C1" s="21" t="s">
+    <row r="1" spans="3:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -728,10 +725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D3810F-B3CD-4F89-AEE8-973E35F9E8B9}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -753,21 +750,21 @@
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="24"/>
+      <c r="C1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="18"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="25"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="26"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="32"/>
+      <c r="M1" s="22"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -777,21 +774,21 @@
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="24"/>
+      <c r="C2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="18"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="26"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="8"/>
-      <c r="K2" s="26"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="33"/>
+      <c r="M2" s="23"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -801,21 +798,21 @@
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="24"/>
+      <c r="C3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="18"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="26"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="8"/>
-      <c r="K3" s="26"/>
+      <c r="K3" s="20"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="33"/>
+      <c r="M3" s="23"/>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -825,21 +822,21 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="24"/>
+      <c r="C4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="18"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="26"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="26"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="33"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -849,21 +846,21 @@
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="24"/>
+      <c r="C5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="26"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="26"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="33"/>
+      <c r="M5" s="23"/>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -873,21 +870,21 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="24"/>
+      <c r="C6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="26"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="26"/>
+      <c r="K6" s="20"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="33"/>
+      <c r="M6" s="23"/>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -897,21 +894,21 @@
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="24"/>
+      <c r="C7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="18"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="26"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="26"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="33"/>
+      <c r="M7" s="23"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -921,21 +918,21 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="24"/>
+      <c r="C8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="18"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="26"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="26"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="33"/>
+      <c r="M8" s="23"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -945,21 +942,21 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="24"/>
+      <c r="C9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="18"/>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="26"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="26"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="33"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -969,21 +966,21 @@
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="24"/>
+      <c r="C10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="18"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="26"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="8"/>
-      <c r="K10" s="26"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="33"/>
+      <c r="M10" s="23"/>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -993,21 +990,21 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="24"/>
+      <c r="C11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="18"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="26"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="26"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="33"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1017,50 +1014,49 @@
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="24"/>
+      <c r="C12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="18"/>
       <c r="F12" s="10"/>
       <c r="G12" s="11"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="27"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="26"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="34"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="C13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="35"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>